<commit_message>
Dodan scenarij i tok događaja za upotrebu aplikacije od strane uposlenika
</commit_message>
<xml_diff>
--- a/UseCaseScenarij/Upotreba aplikacije od strane uposlenika.xlsx
+++ b/UseCaseScenarij/Upotreba aplikacije od strane uposlenika.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Naziv</t>
   </si>
@@ -62,18 +62,243 @@
   </si>
   <si>
     <t>Vozač pogrešno unese podatke, sistem traži ponovni unos podataka./ Vozač obavještava administratora o  problemima i promjenama u saobraćaju, koji dalje te informacije dijeli sa ostalim korisnicima pomoću aplikacije.</t>
+  </si>
+  <si>
+    <t>Glavni tok događaja:</t>
+  </si>
+  <si>
+    <t>Vozač</t>
+  </si>
+  <si>
+    <t>Administrator</t>
+  </si>
+  <si>
+    <r>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pristupanje interfejsu aplikacije</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Unošenje sigurnosnog koda</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Validacija sigurnosnog koda</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Unošenje sigurnosnog koda vozila</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Spajanje vozila sa sistemom</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Obavještavanje administratora o stanju na putu</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>8.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Postavljanje informacije na aplikaciju</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">       </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Validacija sigurnosnog koda vozila</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -118,6 +343,20 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -144,7 +383,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -219,43 +458,80 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFill="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" applyNumberFormat="0" applyFill="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" applyFill="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFill="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyNumberFormat="0" applyFill="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" applyFill="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" applyNumberFormat="0" applyProtection="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="2" applyFont="1" applyFill="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -567,10 +843,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,14 +915,87 @@
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
     </row>
+    <row r="10" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5"/>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="8"/>
+    </row>
+    <row r="16" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="8"/>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7"/>
+      <c r="B18" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:2" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="13"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B20:B21"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>